<commit_message>
Update Impact List Query.
</commit_message>
<xml_diff>
--- a/SA_Recommended_DOQL_Import.xlsx
+++ b/SA_Recommended_DOQL_Import.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jason\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jason\Documents\GitHub\DOQL_scripts_examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA86F04C-D1D9-4999-9693-691E832BD66F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B40ED72C-E85B-4138-8FB9-56F1849620C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -860,15 +860,14 @@
   <si>
     <t xml:space="preserve">/* Get report to Support Impact List */
 /* Inline view of  Target service and Device data  - Filters down to just the records needed   
-        Change device_pk_1 or device_pk_2 to the device id of the focused host before running or
-use &amp;device_pk_1=device_id as parameters.         */
+        Change xxxxx or xxxxy to the device id of the focused host before running          */
 With 
     src as (
        Select Distinct
         dev.device_pk,
 		dev.name
        From view_device_v1 as dev
-         Where dev.device_pk IN ('{device_pk_1}', '{device_pk_2}') /* specify device pk - Can put as many entries as long as each one is put in single quotes and separated by a comma  */
+         Where dev.device_pk IN ('365') /* specify device pk - Can put as many entries as long as each one is put in single quotes and separated by a comma  */
     ),	 
      target_host as (
         Select Distinct		   
@@ -1315,7 +1314,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
+      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>